<commit_message>
new commit, dockerscripts added
</commit_message>
<xml_diff>
--- a/TempFiles/hp/hp_sentiment_analysis_final.xlsx
+++ b/TempFiles/hp/hp_sentiment_analysis_final.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C249"/>
+  <dimension ref="A1:C256"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,11 +451,11 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2023-02-12</t>
+          <t>2023-03-01</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0.8555</v>
+        <v>0.4609</v>
       </c>
     </row>
     <row r="3">
@@ -464,11 +464,11 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2023-02-10</t>
+          <t>2023-02-24</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0</v>
+        <v>0.2023</v>
       </c>
     </row>
     <row r="4">
@@ -477,11 +477,11 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2023-02-09</t>
+          <t>2023-02-23</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0.4196</v>
+        <v>0.3185</v>
       </c>
     </row>
     <row r="5">
@@ -490,11 +490,11 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2023-02-07</t>
+          <t>2023-02-22</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.3185</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -503,11 +503,11 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2023-02-03</t>
+          <t>2023-02-21</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>-0.128</v>
+        <v>-0.1759</v>
       </c>
     </row>
     <row r="7">
@@ -516,7 +516,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2023-02-02</t>
+          <t>2023-02-19</t>
         </is>
       </c>
       <c r="C7" t="n">
@@ -529,11 +529,11 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>2023-01-30</t>
+          <t>2023-02-18</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0</v>
+        <v>0.6369</v>
       </c>
     </row>
     <row r="9">
@@ -542,11 +542,11 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>2023-01-29</t>
+          <t>2023-02-12</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>0.3185</v>
+        <v>0.8555</v>
       </c>
     </row>
     <row r="10">
@@ -555,11 +555,11 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>2023-01-28</t>
+          <t>2023-02-10</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>0.6369</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
@@ -568,11 +568,11 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>2023-01-26</t>
+          <t>2023-02-09</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.6369</v>
+        <v>0.4196</v>
       </c>
     </row>
     <row r="12">
@@ -581,11 +581,11 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>2023-01-25</t>
+          <t>2023-02-07</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>0.6369</v>
+        <v>0.3185</v>
       </c>
     </row>
     <row r="13">
@@ -594,11 +594,11 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>2023-01-23</t>
+          <t>2023-02-03</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>0.6369</v>
+        <v>-0.128</v>
       </c>
     </row>
     <row r="14">
@@ -607,7 +607,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>2023-01-22</t>
+          <t>2023-02-02</t>
         </is>
       </c>
       <c r="C14" t="n">
@@ -620,11 +620,11 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>2023-01-21</t>
+          <t>2023-01-30</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>-0.296</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16">
@@ -633,11 +633,11 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>2023-01-20</t>
+          <t>2023-01-29</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>-0.296</v>
+        <v>0.3185</v>
       </c>
     </row>
     <row r="17">
@@ -646,11 +646,11 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>2023-01-19</t>
+          <t>2023-01-28</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>0.3185</v>
+        <v>0.6369</v>
       </c>
     </row>
     <row r="18">
@@ -659,7 +659,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>2023-01-17</t>
+          <t>2023-01-26</t>
         </is>
       </c>
       <c r="C18" t="n">
@@ -672,11 +672,11 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>2023-01-16</t>
+          <t>2023-01-25</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>-0.0258</v>
+        <v>0.6369</v>
       </c>
     </row>
     <row r="20">
@@ -685,11 +685,11 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>2023-01-15</t>
+          <t>2023-01-23</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>0</v>
+        <v>0.6369</v>
       </c>
     </row>
     <row r="21">
@@ -698,11 +698,11 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>2023-01-14</t>
+          <t>2023-01-22</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>0.2533</v>
+        <v>0.6369</v>
       </c>
     </row>
     <row r="22">
@@ -711,11 +711,11 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>2023-01-12</t>
+          <t>2023-01-21</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>0.2793</v>
+        <v>-0.296</v>
       </c>
     </row>
     <row r="23">
@@ -724,11 +724,11 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>2023-01-11</t>
+          <t>2023-01-20</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>0.1012</v>
+        <v>-0.296</v>
       </c>
     </row>
     <row r="24">
@@ -737,11 +737,11 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>2023-01-06</t>
+          <t>2023-01-19</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>0</v>
+        <v>0.3185</v>
       </c>
     </row>
     <row r="25">
@@ -750,11 +750,11 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>2023-01-03</t>
+          <t>2023-01-17</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>0.1931</v>
+        <v>0.6369</v>
       </c>
     </row>
     <row r="26">
@@ -763,11 +763,11 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>2023-01-02</t>
+          <t>2023-01-16</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>0.739</v>
+        <v>-0.0258</v>
       </c>
     </row>
     <row r="27">
@@ -776,11 +776,11 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>2023-01-01</t>
+          <t>2023-01-15</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>0.6369</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28">
@@ -789,11 +789,11 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>2022-12-31</t>
+          <t>2023-01-14</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>0.3185</v>
+        <v>0.2533</v>
       </c>
     </row>
     <row r="29">
@@ -802,11 +802,11 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>2022-12-30</t>
+          <t>2023-01-12</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>0.6825</v>
+        <v>0.2793</v>
       </c>
     </row>
     <row r="30">
@@ -815,11 +815,11 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>2022-12-19</t>
+          <t>2023-01-11</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>0</v>
+        <v>0.1012</v>
       </c>
     </row>
     <row r="31">
@@ -828,11 +828,11 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>2022-12-16</t>
+          <t>2023-01-06</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>0.2023</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32">
@@ -841,11 +841,11 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>2022-12-15</t>
+          <t>2023-01-03</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>0.2263</v>
+        <v>0.1931</v>
       </c>
     </row>
     <row r="33">
@@ -854,11 +854,11 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>2022-12-13</t>
+          <t>2023-01-02</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>0.2023</v>
+        <v>0.739</v>
       </c>
     </row>
     <row r="34">
@@ -867,11 +867,11 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>2022-12-12</t>
+          <t>2023-01-01</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>0.1012</v>
+        <v>0.6369</v>
       </c>
     </row>
     <row r="35">
@@ -880,11 +880,11 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>2022-12-11</t>
+          <t>2022-12-31</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>0.2609</v>
+        <v>0.3185</v>
       </c>
     </row>
     <row r="36">
@@ -893,11 +893,11 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>2022-12-09</t>
+          <t>2022-12-30</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>0.296</v>
+        <v>0.6825</v>
       </c>
     </row>
     <row r="37">
@@ -906,7 +906,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>2022-12-08</t>
+          <t>2022-12-19</t>
         </is>
       </c>
       <c r="C37" t="n">
@@ -919,11 +919,11 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>2022-12-07</t>
+          <t>2022-12-16</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>0</v>
+        <v>0.2023</v>
       </c>
     </row>
     <row r="39">
@@ -932,11 +932,11 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>2022-12-04</t>
+          <t>2022-12-15</t>
         </is>
       </c>
       <c r="C39" t="n">
-        <v>0.2732</v>
+        <v>0.2263</v>
       </c>
     </row>
     <row r="40">
@@ -945,11 +945,11 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>2022-12-03</t>
+          <t>2022-12-13</t>
         </is>
       </c>
       <c r="C40" t="n">
-        <v>0.6249</v>
+        <v>0.2023</v>
       </c>
     </row>
     <row r="41">
@@ -958,11 +958,11 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>2022-12-01</t>
+          <t>2022-12-12</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>-0.3818</v>
+        <v>0.1012</v>
       </c>
     </row>
     <row r="42">
@@ -971,11 +971,11 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>2022-11-30</t>
+          <t>2022-12-11</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>0.2023</v>
+        <v>0.2609</v>
       </c>
     </row>
     <row r="43">
@@ -984,11 +984,11 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>2022-11-29</t>
+          <t>2022-12-09</t>
         </is>
       </c>
       <c r="C43" t="n">
-        <v>0</v>
+        <v>0.296</v>
       </c>
     </row>
     <row r="44">
@@ -997,7 +997,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>2022-11-27</t>
+          <t>2022-12-08</t>
         </is>
       </c>
       <c r="C44" t="n">
@@ -1010,7 +1010,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>2022-11-26</t>
+          <t>2022-12-07</t>
         </is>
       </c>
       <c r="C45" t="n">
@@ -1023,11 +1023,11 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>2022-11-24</t>
+          <t>2022-12-04</t>
         </is>
       </c>
       <c r="C46" t="n">
-        <v>0.2038</v>
+        <v>0.2732</v>
       </c>
     </row>
     <row r="47">
@@ -1036,11 +1036,11 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>2022-11-23</t>
+          <t>2022-12-03</t>
         </is>
       </c>
       <c r="C47" t="n">
-        <v>0.1781</v>
+        <v>0.6249</v>
       </c>
     </row>
     <row r="48">
@@ -1049,11 +1049,11 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>2022-11-22</t>
+          <t>2022-12-01</t>
         </is>
       </c>
       <c r="C48" t="n">
-        <v>0</v>
+        <v>-0.3818</v>
       </c>
     </row>
     <row r="49">
@@ -1062,11 +1062,11 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>2022-11-21</t>
+          <t>2022-11-30</t>
         </is>
       </c>
       <c r="C49" t="n">
-        <v>-0.0453</v>
+        <v>0.2023</v>
       </c>
     </row>
     <row r="50">
@@ -1075,7 +1075,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>2022-11-20</t>
+          <t>2022-11-29</t>
         </is>
       </c>
       <c r="C50" t="n">
@@ -1088,7 +1088,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>2022-11-19</t>
+          <t>2022-11-27</t>
         </is>
       </c>
       <c r="C51" t="n">
@@ -1101,11 +1101,11 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>2022-11-18</t>
+          <t>2022-11-26</t>
         </is>
       </c>
       <c r="C52" t="n">
-        <v>0.2023</v>
+        <v>0</v>
       </c>
     </row>
     <row r="53">
@@ -1114,11 +1114,11 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>2022-11-17</t>
+          <t>2022-11-24</t>
         </is>
       </c>
       <c r="C53" t="n">
-        <v>0.2715</v>
+        <v>0.2038</v>
       </c>
     </row>
     <row r="54">
@@ -1127,11 +1127,11 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>2022-11-16</t>
+          <t>2022-11-23</t>
         </is>
       </c>
       <c r="C54" t="n">
-        <v>0</v>
+        <v>0.1781</v>
       </c>
     </row>
     <row r="55">
@@ -1140,11 +1140,11 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>2022-11-15</t>
+          <t>2022-11-22</t>
         </is>
       </c>
       <c r="C55" t="n">
-        <v>-0.296</v>
+        <v>0</v>
       </c>
     </row>
     <row r="56">
@@ -1153,11 +1153,11 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>2022-11-14</t>
+          <t>2022-11-21</t>
         </is>
       </c>
       <c r="C56" t="n">
-        <v>-0.1909</v>
+        <v>-0.0453</v>
       </c>
     </row>
     <row r="57">
@@ -1166,11 +1166,11 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>2022-11-13</t>
+          <t>2022-11-20</t>
         </is>
       </c>
       <c r="C57" t="n">
-        <v>0.1147</v>
+        <v>0</v>
       </c>
     </row>
     <row r="58">
@@ -1179,7 +1179,7 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>2022-11-12</t>
+          <t>2022-11-19</t>
         </is>
       </c>
       <c r="C58" t="n">
@@ -1192,11 +1192,11 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>2022-11-11</t>
+          <t>2022-11-18</t>
         </is>
       </c>
       <c r="C59" t="n">
-        <v>0</v>
+        <v>0.2023</v>
       </c>
     </row>
     <row r="60">
@@ -1205,11 +1205,11 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>2022-11-03</t>
+          <t>2022-11-17</t>
         </is>
       </c>
       <c r="C60" t="n">
-        <v>0</v>
+        <v>0.2715</v>
       </c>
     </row>
     <row r="61">
@@ -1218,11 +1218,11 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>2022-11-01</t>
+          <t>2022-11-16</t>
         </is>
       </c>
       <c r="C61" t="n">
-        <v>0.2023</v>
+        <v>0</v>
       </c>
     </row>
     <row r="62">
@@ -1231,11 +1231,11 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>2022-10-28</t>
+          <t>2022-11-15</t>
         </is>
       </c>
       <c r="C62" t="n">
-        <v>0</v>
+        <v>-0.296</v>
       </c>
     </row>
     <row r="63">
@@ -1244,11 +1244,11 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>2022-10-27</t>
+          <t>2022-11-14</t>
         </is>
       </c>
       <c r="C63" t="n">
-        <v>0</v>
+        <v>-0.1909</v>
       </c>
     </row>
     <row r="64">
@@ -1257,11 +1257,11 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>2022-10-26</t>
+          <t>2022-11-13</t>
         </is>
       </c>
       <c r="C64" t="n">
-        <v>0.0506</v>
+        <v>0.1147</v>
       </c>
     </row>
     <row r="65">
@@ -1270,7 +1270,7 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>2022-10-25</t>
+          <t>2022-11-12</t>
         </is>
       </c>
       <c r="C65" t="n">
@@ -1283,11 +1283,11 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>2022-10-21</t>
+          <t>2022-11-11</t>
         </is>
       </c>
       <c r="C66" t="n">
-        <v>0.2023</v>
+        <v>0</v>
       </c>
     </row>
     <row r="67">
@@ -1296,7 +1296,7 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>2022-10-20</t>
+          <t>2022-11-03</t>
         </is>
       </c>
       <c r="C67" t="n">
@@ -1309,11 +1309,11 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>2022-10-19</t>
+          <t>2022-11-01</t>
         </is>
       </c>
       <c r="C68" t="n">
-        <v>0</v>
+        <v>0.2023</v>
       </c>
     </row>
     <row r="69">
@@ -1322,7 +1322,7 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>2022-10-17</t>
+          <t>2022-10-28</t>
         </is>
       </c>
       <c r="C69" t="n">
@@ -1335,7 +1335,7 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>2022-10-13</t>
+          <t>2022-10-27</t>
         </is>
       </c>
       <c r="C70" t="n">
@@ -1348,11 +1348,11 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>2022-10-10</t>
+          <t>2022-10-26</t>
         </is>
       </c>
       <c r="C71" t="n">
-        <v>-0.128</v>
+        <v>0.0506</v>
       </c>
     </row>
     <row r="72">
@@ -1361,11 +1361,11 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>2022-10-07</t>
+          <t>2022-10-25</t>
         </is>
       </c>
       <c r="C72" t="n">
-        <v>0.3375</v>
+        <v>0</v>
       </c>
     </row>
     <row r="73">
@@ -1374,11 +1374,11 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>2022-10-05</t>
+          <t>2022-10-21</t>
         </is>
       </c>
       <c r="C73" t="n">
-        <v>0</v>
+        <v>0.2023</v>
       </c>
     </row>
     <row r="74">
@@ -1387,11 +1387,11 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>2022-10-04</t>
+          <t>2022-10-20</t>
         </is>
       </c>
       <c r="C74" t="n">
-        <v>0.2023</v>
+        <v>0</v>
       </c>
     </row>
     <row r="75">
@@ -1400,11 +1400,11 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>2022-10-02</t>
+          <t>2022-10-19</t>
         </is>
       </c>
       <c r="C75" t="n">
-        <v>0.2108</v>
+        <v>0</v>
       </c>
     </row>
     <row r="76">
@@ -1413,11 +1413,11 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>2022-09-27</t>
+          <t>2022-10-17</t>
         </is>
       </c>
       <c r="C76" t="n">
-        <v>0.1012</v>
+        <v>0</v>
       </c>
     </row>
     <row r="77">
@@ -1426,11 +1426,11 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>2022-09-25</t>
+          <t>2022-10-13</t>
         </is>
       </c>
       <c r="C77" t="n">
-        <v>0.296</v>
+        <v>0</v>
       </c>
     </row>
     <row r="78">
@@ -1439,11 +1439,11 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>2022-09-23</t>
+          <t>2022-10-10</t>
         </is>
       </c>
       <c r="C78" t="n">
-        <v>0.0757</v>
+        <v>-0.128</v>
       </c>
     </row>
     <row r="79">
@@ -1452,11 +1452,11 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>2022-09-22</t>
+          <t>2022-10-07</t>
         </is>
       </c>
       <c r="C79" t="n">
-        <v>0.1007</v>
+        <v>0.3375</v>
       </c>
     </row>
     <row r="80">
@@ -1465,11 +1465,11 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>2022-09-21</t>
+          <t>2022-10-05</t>
         </is>
       </c>
       <c r="C80" t="n">
-        <v>-0.4184</v>
+        <v>0</v>
       </c>
     </row>
     <row r="81">
@@ -1478,11 +1478,11 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>2022-09-19</t>
+          <t>2022-10-04</t>
         </is>
       </c>
       <c r="C81" t="n">
-        <v>0</v>
+        <v>0.2023</v>
       </c>
     </row>
     <row r="82">
@@ -1491,11 +1491,11 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>2022-09-15</t>
+          <t>2022-10-02</t>
         </is>
       </c>
       <c r="C82" t="n">
-        <v>0.1012</v>
+        <v>0.2108</v>
       </c>
     </row>
     <row r="83">
@@ -1504,11 +1504,11 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>2022-09-14</t>
+          <t>2022-09-27</t>
         </is>
       </c>
       <c r="C83" t="n">
-        <v>0</v>
+        <v>0.1012</v>
       </c>
     </row>
     <row r="84">
@@ -1517,11 +1517,11 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>2022-09-13</t>
+          <t>2022-09-25</t>
         </is>
       </c>
       <c r="C84" t="n">
-        <v>0.2023</v>
+        <v>0.296</v>
       </c>
     </row>
     <row r="85">
@@ -1530,11 +1530,11 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>2022-09-11</t>
+          <t>2022-09-23</t>
         </is>
       </c>
       <c r="C85" t="n">
-        <v>0</v>
+        <v>0.0757</v>
       </c>
     </row>
     <row r="86">
@@ -1543,11 +1543,11 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>2022-09-07</t>
+          <t>2022-09-22</t>
         </is>
       </c>
       <c r="C86" t="n">
-        <v>0</v>
+        <v>0.1007</v>
       </c>
     </row>
     <row r="87">
@@ -1556,11 +1556,11 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>2022-09-06</t>
+          <t>2022-09-21</t>
         </is>
       </c>
       <c r="C87" t="n">
-        <v>0.0361</v>
+        <v>-0.4184</v>
       </c>
     </row>
     <row r="88">
@@ -1569,11 +1569,11 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>2022-09-02</t>
+          <t>2022-09-19</t>
         </is>
       </c>
       <c r="C88" t="n">
-        <v>0.3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="89">
@@ -1582,11 +1582,11 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>2022-09-01</t>
+          <t>2022-09-15</t>
         </is>
       </c>
       <c r="C89" t="n">
-        <v>0.1517</v>
+        <v>0.1012</v>
       </c>
     </row>
     <row r="90">
@@ -1595,11 +1595,11 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>2022-08-31</t>
+          <t>2022-09-14</t>
         </is>
       </c>
       <c r="C90" t="n">
-        <v>0.1517</v>
+        <v>0</v>
       </c>
     </row>
     <row r="91">
@@ -1608,11 +1608,11 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>2022-08-30</t>
+          <t>2022-09-13</t>
         </is>
       </c>
       <c r="C91" t="n">
-        <v>0.0326</v>
+        <v>0.2023</v>
       </c>
     </row>
     <row r="92">
@@ -1621,7 +1621,7 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>2022-08-29</t>
+          <t>2022-09-11</t>
         </is>
       </c>
       <c r="C92" t="n">
@@ -1634,11 +1634,11 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>2022-08-28</t>
+          <t>2022-09-07</t>
         </is>
       </c>
       <c r="C93" t="n">
-        <v>-0.0465</v>
+        <v>0</v>
       </c>
     </row>
     <row r="94">
@@ -1647,11 +1647,11 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>2022-08-27</t>
+          <t>2022-09-06</t>
         </is>
       </c>
       <c r="C94" t="n">
-        <v>0.5461</v>
+        <v>0.0361</v>
       </c>
     </row>
     <row r="95">
@@ -1660,11 +1660,11 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>2022-08-26</t>
+          <t>2022-09-02</t>
         </is>
       </c>
       <c r="C95" t="n">
-        <v>0.1929</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="96">
@@ -1673,11 +1673,11 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>2022-08-25</t>
+          <t>2022-09-01</t>
         </is>
       </c>
       <c r="C96" t="n">
-        <v>-0.1589</v>
+        <v>0.1517</v>
       </c>
     </row>
     <row r="97">
@@ -1686,11 +1686,11 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>2022-08-24</t>
+          <t>2022-08-31</t>
         </is>
       </c>
       <c r="C97" t="n">
-        <v>0.5461</v>
+        <v>0.1517</v>
       </c>
     </row>
     <row r="98">
@@ -1699,11 +1699,11 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>2022-08-22</t>
+          <t>2022-08-30</t>
         </is>
       </c>
       <c r="C98" t="n">
-        <v>0.4019</v>
+        <v>0.0326</v>
       </c>
     </row>
     <row r="99">
@@ -1712,7 +1712,7 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>2022-08-20</t>
+          <t>2022-08-29</t>
         </is>
       </c>
       <c r="C99" t="n">
@@ -1725,11 +1725,11 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>2022-08-17</t>
+          <t>2022-08-28</t>
         </is>
       </c>
       <c r="C100" t="n">
-        <v>0.594</v>
+        <v>-0.0465</v>
       </c>
     </row>
     <row r="101">
@@ -1738,11 +1738,11 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>2022-08-16</t>
+          <t>2022-08-27</t>
         </is>
       </c>
       <c r="C101" t="n">
-        <v>0</v>
+        <v>0.5461</v>
       </c>
     </row>
     <row r="102">
@@ -1751,11 +1751,11 @@
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>2022-08-15</t>
+          <t>2022-08-26</t>
         </is>
       </c>
       <c r="C102" t="n">
-        <v>0</v>
+        <v>0.1929</v>
       </c>
     </row>
     <row r="103">
@@ -1764,11 +1764,11 @@
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>2022-08-12</t>
+          <t>2022-08-25</t>
         </is>
       </c>
       <c r="C103" t="n">
-        <v>0.1618</v>
+        <v>-0.1589</v>
       </c>
     </row>
     <row r="104">
@@ -1777,11 +1777,11 @@
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>2022-08-11</t>
+          <t>2022-08-24</t>
         </is>
       </c>
       <c r="C104" t="n">
-        <v>0</v>
+        <v>0.5461</v>
       </c>
     </row>
     <row r="105">
@@ -1790,11 +1790,11 @@
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>2022-08-10</t>
+          <t>2022-08-22</t>
         </is>
       </c>
       <c r="C105" t="n">
-        <v>0.2023</v>
+        <v>0.4019</v>
       </c>
     </row>
     <row r="106">
@@ -1803,11 +1803,11 @@
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>2022-07-27</t>
+          <t>2022-08-20</t>
         </is>
       </c>
       <c r="C106" t="n">
-        <v>0.0397</v>
+        <v>0</v>
       </c>
     </row>
     <row r="107">
@@ -1816,11 +1816,11 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>2022-07-26</t>
+          <t>2022-08-17</t>
         </is>
       </c>
       <c r="C107" t="n">
-        <v>0.1007</v>
+        <v>0.594</v>
       </c>
     </row>
     <row r="108">
@@ -1829,11 +1829,11 @@
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>2022-07-25</t>
+          <t>2022-08-16</t>
         </is>
       </c>
       <c r="C108" t="n">
-        <v>-0.4184</v>
+        <v>0</v>
       </c>
     </row>
     <row r="109">
@@ -1842,11 +1842,11 @@
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>2022-07-24</t>
+          <t>2022-08-15</t>
         </is>
       </c>
       <c r="C109" t="n">
-        <v>-0.0723</v>
+        <v>0</v>
       </c>
     </row>
     <row r="110">
@@ -1855,11 +1855,11 @@
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>2022-07-23</t>
+          <t>2022-08-12</t>
         </is>
       </c>
       <c r="C110" t="n">
-        <v>-0.1589</v>
+        <v>0.1618</v>
       </c>
     </row>
     <row r="111">
@@ -1868,11 +1868,11 @@
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>2022-07-22</t>
+          <t>2022-08-11</t>
         </is>
       </c>
       <c r="C111" t="n">
-        <v>0.1007</v>
+        <v>0</v>
       </c>
     </row>
     <row r="112">
@@ -1881,7 +1881,7 @@
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>2022-07-21</t>
+          <t>2022-08-10</t>
         </is>
       </c>
       <c r="C112" t="n">
@@ -1894,11 +1894,11 @@
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>2022-07-20</t>
+          <t>2022-07-27</t>
         </is>
       </c>
       <c r="C113" t="n">
-        <v>-0.5837</v>
+        <v>0.0397</v>
       </c>
     </row>
     <row r="114">
@@ -1907,11 +1907,11 @@
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>2022-07-19</t>
+          <t>2022-07-26</t>
         </is>
       </c>
       <c r="C114" t="n">
-        <v>-0.1081</v>
+        <v>0.1007</v>
       </c>
     </row>
     <row r="115">
@@ -1920,11 +1920,11 @@
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>2022-07-18</t>
+          <t>2022-07-25</t>
         </is>
       </c>
       <c r="C115" t="n">
-        <v>-0.0162</v>
+        <v>-0.4184</v>
       </c>
     </row>
     <row r="116">
@@ -1933,11 +1933,11 @@
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>2022-07-17</t>
+          <t>2022-07-24</t>
         </is>
       </c>
       <c r="C116" t="n">
-        <v>0.1007</v>
+        <v>-0.0723</v>
       </c>
     </row>
     <row r="117">
@@ -1946,11 +1946,11 @@
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>2022-07-16</t>
+          <t>2022-07-23</t>
         </is>
       </c>
       <c r="C117" t="n">
-        <v>-0.1586</v>
+        <v>-0.1589</v>
       </c>
     </row>
     <row r="118">
@@ -1959,11 +1959,11 @@
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>2022-07-15</t>
+          <t>2022-07-22</t>
         </is>
       </c>
       <c r="C118" t="n">
-        <v>0.0674</v>
+        <v>0.1007</v>
       </c>
     </row>
     <row r="119">
@@ -1972,11 +1972,11 @@
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>2022-07-14</t>
+          <t>2022-07-21</t>
         </is>
       </c>
       <c r="C119" t="n">
-        <v>-0.4082</v>
+        <v>0.2023</v>
       </c>
     </row>
     <row r="120">
@@ -1985,11 +1985,11 @@
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>2022-07-13</t>
+          <t>2022-07-20</t>
         </is>
       </c>
       <c r="C120" t="n">
-        <v>-0.0263</v>
+        <v>-0.5837</v>
       </c>
     </row>
     <row r="121">
@@ -1998,11 +1998,11 @@
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>2022-07-11</t>
+          <t>2022-07-19</t>
         </is>
       </c>
       <c r="C121" t="n">
-        <v>0.1684</v>
+        <v>-0.1081</v>
       </c>
     </row>
     <row r="122">
@@ -2011,11 +2011,11 @@
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>2022-07-09</t>
+          <t>2022-07-18</t>
         </is>
       </c>
       <c r="C122" t="n">
-        <v>-0.1589</v>
+        <v>-0.0162</v>
       </c>
     </row>
     <row r="123">
@@ -2024,7 +2024,7 @@
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>2022-07-08</t>
+          <t>2022-07-17</t>
         </is>
       </c>
       <c r="C123" t="n">
@@ -2037,11 +2037,11 @@
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>2022-07-06</t>
+          <t>2022-07-16</t>
         </is>
       </c>
       <c r="C124" t="n">
-        <v>-0.1059</v>
+        <v>-0.1586</v>
       </c>
     </row>
     <row r="125">
@@ -2050,11 +2050,11 @@
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>2022-07-05</t>
+          <t>2022-07-15</t>
         </is>
       </c>
       <c r="C125" t="n">
-        <v>0.075</v>
+        <v>0.0674</v>
       </c>
     </row>
     <row r="126">
@@ -2063,11 +2063,11 @@
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>2022-07-02</t>
+          <t>2022-07-14</t>
         </is>
       </c>
       <c r="C126" t="n">
-        <v>-0.4184</v>
+        <v>-0.4082</v>
       </c>
     </row>
     <row r="127">
@@ -2076,11 +2076,11 @@
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>2022-07-01</t>
+          <t>2022-07-13</t>
         </is>
       </c>
       <c r="C127" t="n">
-        <v>-0.1586</v>
+        <v>-0.0263</v>
       </c>
     </row>
     <row r="128">
@@ -2089,11 +2089,11 @@
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>2022-06-30</t>
+          <t>2022-07-11</t>
         </is>
       </c>
       <c r="C128" t="n">
-        <v>0.0098</v>
+        <v>0.1684</v>
       </c>
     </row>
     <row r="129">
@@ -2102,11 +2102,11 @@
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>2022-06-29</t>
+          <t>2022-07-09</t>
         </is>
       </c>
       <c r="C129" t="n">
-        <v>0.0154</v>
+        <v>-0.1589</v>
       </c>
     </row>
     <row r="130">
@@ -2115,11 +2115,11 @@
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>2022-06-28</t>
+          <t>2022-07-08</t>
         </is>
       </c>
       <c r="C130" t="n">
-        <v>0.0449</v>
+        <v>0.1007</v>
       </c>
     </row>
     <row r="131">
@@ -2128,11 +2128,11 @@
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>2022-06-27</t>
+          <t>2022-07-06</t>
         </is>
       </c>
       <c r="C131" t="n">
-        <v>0.1007</v>
+        <v>-0.1059</v>
       </c>
     </row>
     <row r="132">
@@ -2141,11 +2141,11 @@
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>2022-06-26</t>
+          <t>2022-07-05</t>
         </is>
       </c>
       <c r="C132" t="n">
-        <v>0.1007</v>
+        <v>0.075</v>
       </c>
     </row>
     <row r="133">
@@ -2154,11 +2154,11 @@
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>2022-06-25</t>
+          <t>2022-07-02</t>
         </is>
       </c>
       <c r="C133" t="n">
-        <v>0.0489</v>
+        <v>-0.4184</v>
       </c>
     </row>
     <row r="134">
@@ -2167,11 +2167,11 @@
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>2022-06-24</t>
+          <t>2022-07-01</t>
         </is>
       </c>
       <c r="C134" t="n">
-        <v>0.0429</v>
+        <v>-0.1586</v>
       </c>
     </row>
     <row r="135">
@@ -2180,11 +2180,11 @@
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>2022-06-23</t>
+          <t>2022-06-30</t>
         </is>
       </c>
       <c r="C135" t="n">
-        <v>-0.166</v>
+        <v>0.0098</v>
       </c>
     </row>
     <row r="136">
@@ -2193,11 +2193,11 @@
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>2022-06-22</t>
+          <t>2022-06-29</t>
         </is>
       </c>
       <c r="C136" t="n">
-        <v>-0.0424</v>
+        <v>0.0154</v>
       </c>
     </row>
     <row r="137">
@@ -2206,11 +2206,11 @@
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>2022-06-21</t>
+          <t>2022-06-28</t>
         </is>
       </c>
       <c r="C137" t="n">
-        <v>0.0516</v>
+        <v>0.0449</v>
       </c>
     </row>
     <row r="138">
@@ -2219,11 +2219,11 @@
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>2022-06-19</t>
+          <t>2022-06-27</t>
         </is>
       </c>
       <c r="C138" t="n">
-        <v>-0.1351</v>
+        <v>0.1007</v>
       </c>
     </row>
     <row r="139">
@@ -2232,11 +2232,11 @@
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>2022-06-18</t>
+          <t>2022-06-26</t>
         </is>
       </c>
       <c r="C139" t="n">
-        <v>-0.0033</v>
+        <v>0.1007</v>
       </c>
     </row>
     <row r="140">
@@ -2245,11 +2245,11 @@
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>2022-06-17</t>
+          <t>2022-06-25</t>
         </is>
       </c>
       <c r="C140" t="n">
-        <v>0.1141</v>
+        <v>0.0489</v>
       </c>
     </row>
     <row r="141">
@@ -2258,11 +2258,11 @@
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>2022-06-16</t>
+          <t>2022-06-24</t>
         </is>
       </c>
       <c r="C141" t="n">
-        <v>0.1055</v>
+        <v>0.0429</v>
       </c>
     </row>
     <row r="142">
@@ -2271,11 +2271,11 @@
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>2022-06-15</t>
+          <t>2022-06-23</t>
         </is>
       </c>
       <c r="C142" t="n">
-        <v>0.1012</v>
+        <v>-0.166</v>
       </c>
     </row>
     <row r="143">
@@ -2284,11 +2284,11 @@
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>2022-06-14</t>
+          <t>2022-06-22</t>
         </is>
       </c>
       <c r="C143" t="n">
-        <v>-0.0312</v>
+        <v>-0.0424</v>
       </c>
     </row>
     <row r="144">
@@ -2297,11 +2297,11 @@
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>2022-06-13</t>
+          <t>2022-06-21</t>
         </is>
       </c>
       <c r="C144" t="n">
-        <v>0.2023</v>
+        <v>0.0516</v>
       </c>
     </row>
     <row r="145">
@@ -2310,7 +2310,7 @@
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>2022-06-12</t>
+          <t>2022-06-19</t>
         </is>
       </c>
       <c r="C145" t="n">
@@ -2323,11 +2323,11 @@
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>2022-06-11</t>
+          <t>2022-06-18</t>
         </is>
       </c>
       <c r="C146" t="n">
-        <v>-0.2345</v>
+        <v>-0.0033</v>
       </c>
     </row>
     <row r="147">
@@ -2336,11 +2336,11 @@
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>2022-06-10</t>
+          <t>2022-06-17</t>
         </is>
       </c>
       <c r="C147" t="n">
-        <v>0.0129</v>
+        <v>0.1141</v>
       </c>
     </row>
     <row r="148">
@@ -2349,11 +2349,11 @@
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>2022-06-09</t>
+          <t>2022-06-16</t>
         </is>
       </c>
       <c r="C148" t="n">
-        <v>-0.1776</v>
+        <v>0.1055</v>
       </c>
     </row>
     <row r="149">
@@ -2362,11 +2362,11 @@
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>2022-06-08</t>
+          <t>2022-06-15</t>
         </is>
       </c>
       <c r="C149" t="n">
-        <v>0</v>
+        <v>0.1012</v>
       </c>
     </row>
     <row r="150">
@@ -2375,11 +2375,11 @@
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>2022-06-07</t>
+          <t>2022-06-14</t>
         </is>
       </c>
       <c r="C150" t="n">
-        <v>0</v>
+        <v>-0.0312</v>
       </c>
     </row>
     <row r="151">
@@ -2388,11 +2388,11 @@
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>2022-06-05</t>
+          <t>2022-06-13</t>
         </is>
       </c>
       <c r="C151" t="n">
-        <v>0</v>
+        <v>0.2023</v>
       </c>
     </row>
     <row r="152">
@@ -2401,11 +2401,11 @@
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>2022-06-04</t>
+          <t>2022-06-12</t>
         </is>
       </c>
       <c r="C152" t="n">
-        <v>0.2553</v>
+        <v>-0.1351</v>
       </c>
     </row>
     <row r="153">
@@ -2414,11 +2414,11 @@
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>2022-06-03</t>
+          <t>2022-06-11</t>
         </is>
       </c>
       <c r="C153" t="n">
-        <v>0.2023</v>
+        <v>-0.2345</v>
       </c>
     </row>
     <row r="154">
@@ -2427,11 +2427,11 @@
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>2022-06-02</t>
+          <t>2022-06-10</t>
         </is>
       </c>
       <c r="C154" t="n">
-        <v>0.183</v>
+        <v>0.0129</v>
       </c>
     </row>
     <row r="155">
@@ -2440,11 +2440,11 @@
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>2022-06-01</t>
+          <t>2022-06-09</t>
         </is>
       </c>
       <c r="C155" t="n">
-        <v>0.2553</v>
+        <v>-0.1776</v>
       </c>
     </row>
     <row r="156">
@@ -2453,7 +2453,7 @@
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>2022-05-31</t>
+          <t>2022-06-08</t>
         </is>
       </c>
       <c r="C156" t="n">
@@ -2466,7 +2466,7 @@
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>2022-05-30</t>
+          <t>2022-06-07</t>
         </is>
       </c>
       <c r="C157" t="n">
@@ -2479,7 +2479,7 @@
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>2022-05-28</t>
+          <t>2022-06-05</t>
         </is>
       </c>
       <c r="C158" t="n">
@@ -2492,11 +2492,11 @@
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>2022-05-27</t>
+          <t>2022-06-04</t>
         </is>
       </c>
       <c r="C159" t="n">
-        <v>-0.0151</v>
+        <v>0.2553</v>
       </c>
     </row>
     <row r="160">
@@ -2505,11 +2505,11 @@
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>2022-05-26</t>
+          <t>2022-06-03</t>
         </is>
       </c>
       <c r="C160" t="n">
-        <v>0.4404</v>
+        <v>0.2023</v>
       </c>
     </row>
     <row r="161">
@@ -2518,11 +2518,11 @@
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>2022-05-20</t>
+          <t>2022-06-02</t>
         </is>
       </c>
       <c r="C161" t="n">
-        <v>0.2023</v>
+        <v>0.183</v>
       </c>
     </row>
     <row r="162">
@@ -2531,11 +2531,11 @@
       </c>
       <c r="B162" t="inlineStr">
         <is>
-          <t>2022-05-19</t>
+          <t>2022-06-01</t>
         </is>
       </c>
       <c r="C162" t="n">
-        <v>0.2688</v>
+        <v>0.2553</v>
       </c>
     </row>
     <row r="163">
@@ -2544,7 +2544,7 @@
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>2022-05-18</t>
+          <t>2022-05-31</t>
         </is>
       </c>
       <c r="C163" t="n">
@@ -2557,11 +2557,11 @@
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>2022-05-16</t>
+          <t>2022-05-30</t>
         </is>
       </c>
       <c r="C164" t="n">
-        <v>0.2732</v>
+        <v>0</v>
       </c>
     </row>
     <row r="165">
@@ -2570,7 +2570,7 @@
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>2022-05-13</t>
+          <t>2022-05-28</t>
         </is>
       </c>
       <c r="C165" t="n">
@@ -2583,11 +2583,11 @@
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>2022-05-12</t>
+          <t>2022-05-27</t>
         </is>
       </c>
       <c r="C166" t="n">
-        <v>0</v>
+        <v>-0.0151</v>
       </c>
     </row>
     <row r="167">
@@ -2596,11 +2596,11 @@
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>2022-05-08</t>
+          <t>2022-05-26</t>
         </is>
       </c>
       <c r="C167" t="n">
-        <v>0</v>
+        <v>0.4404</v>
       </c>
     </row>
     <row r="168">
@@ -2609,11 +2609,11 @@
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>2022-05-05</t>
+          <t>2022-05-20</t>
         </is>
       </c>
       <c r="C168" t="n">
-        <v>0</v>
+        <v>0.2023</v>
       </c>
     </row>
     <row r="169">
@@ -2622,11 +2622,11 @@
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>2022-05-04</t>
+          <t>2022-05-19</t>
         </is>
       </c>
       <c r="C169" t="n">
-        <v>0</v>
+        <v>0.2688</v>
       </c>
     </row>
     <row r="170">
@@ -2635,11 +2635,11 @@
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>2022-05-03</t>
+          <t>2022-05-18</t>
         </is>
       </c>
       <c r="C170" t="n">
-        <v>0.1227</v>
+        <v>0</v>
       </c>
     </row>
     <row r="171">
@@ -2648,11 +2648,11 @@
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>2022-04-29</t>
+          <t>2022-05-16</t>
         </is>
       </c>
       <c r="C171" t="n">
-        <v>0.2453</v>
+        <v>0.2732</v>
       </c>
     </row>
     <row r="172">
@@ -2661,11 +2661,11 @@
       </c>
       <c r="B172" t="inlineStr">
         <is>
-          <t>2022-04-28</t>
+          <t>2022-05-13</t>
         </is>
       </c>
       <c r="C172" t="n">
-        <v>0.1472</v>
+        <v>0</v>
       </c>
     </row>
     <row r="173">
@@ -2674,11 +2674,11 @@
       </c>
       <c r="B173" t="inlineStr">
         <is>
-          <t>2022-04-27</t>
+          <t>2022-05-12</t>
         </is>
       </c>
       <c r="C173" t="n">
-        <v>0.1012</v>
+        <v>0</v>
       </c>
     </row>
     <row r="174">
@@ -2687,7 +2687,7 @@
       </c>
       <c r="B174" t="inlineStr">
         <is>
-          <t>2022-04-26</t>
+          <t>2022-05-08</t>
         </is>
       </c>
       <c r="C174" t="n">
@@ -2700,7 +2700,7 @@
       </c>
       <c r="B175" t="inlineStr">
         <is>
-          <t>2022-04-23</t>
+          <t>2022-05-05</t>
         </is>
       </c>
       <c r="C175" t="n">
@@ -2713,11 +2713,11 @@
       </c>
       <c r="B176" t="inlineStr">
         <is>
-          <t>2022-04-22</t>
+          <t>2022-05-04</t>
         </is>
       </c>
       <c r="C176" t="n">
-        <v>0.1005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="177">
@@ -2726,11 +2726,11 @@
       </c>
       <c r="B177" t="inlineStr">
         <is>
-          <t>2022-04-21</t>
+          <t>2022-05-03</t>
         </is>
       </c>
       <c r="C177" t="n">
-        <v>0</v>
+        <v>0.1227</v>
       </c>
     </row>
     <row r="178">
@@ -2739,11 +2739,11 @@
       </c>
       <c r="B178" t="inlineStr">
         <is>
-          <t>2022-04-19</t>
+          <t>2022-04-29</t>
         </is>
       </c>
       <c r="C178" t="n">
-        <v>0</v>
+        <v>0.2453</v>
       </c>
     </row>
     <row r="179">
@@ -2752,11 +2752,11 @@
       </c>
       <c r="B179" t="inlineStr">
         <is>
-          <t>2022-04-18</t>
+          <t>2022-04-28</t>
         </is>
       </c>
       <c r="C179" t="n">
-        <v>0</v>
+        <v>0.1472</v>
       </c>
     </row>
     <row r="180">
@@ -2765,11 +2765,11 @@
       </c>
       <c r="B180" t="inlineStr">
         <is>
-          <t>2022-04-17</t>
+          <t>2022-04-27</t>
         </is>
       </c>
       <c r="C180" t="n">
-        <v>0</v>
+        <v>0.1012</v>
       </c>
     </row>
     <row r="181">
@@ -2778,7 +2778,7 @@
       </c>
       <c r="B181" t="inlineStr">
         <is>
-          <t>2022-04-14</t>
+          <t>2022-04-26</t>
         </is>
       </c>
       <c r="C181" t="n">
@@ -2791,11 +2791,11 @@
       </c>
       <c r="B182" t="inlineStr">
         <is>
-          <t>2022-04-12</t>
+          <t>2022-04-23</t>
         </is>
       </c>
       <c r="C182" t="n">
-        <v>0.1198</v>
+        <v>0</v>
       </c>
     </row>
     <row r="183">
@@ -2804,11 +2804,11 @@
       </c>
       <c r="B183" t="inlineStr">
         <is>
-          <t>2022-04-10</t>
+          <t>2022-04-22</t>
         </is>
       </c>
       <c r="C183" t="n">
-        <v>0</v>
+        <v>0.1005</v>
       </c>
     </row>
     <row r="184">
@@ -2817,11 +2817,11 @@
       </c>
       <c r="B184" t="inlineStr">
         <is>
-          <t>2022-04-08</t>
+          <t>2022-04-21</t>
         </is>
       </c>
       <c r="C184" t="n">
-        <v>0.1394</v>
+        <v>0</v>
       </c>
     </row>
     <row r="185">
@@ -2830,7 +2830,7 @@
       </c>
       <c r="B185" t="inlineStr">
         <is>
-          <t>2022-04-07</t>
+          <t>2022-04-19</t>
         </is>
       </c>
       <c r="C185" t="n">
@@ -2843,7 +2843,7 @@
       </c>
       <c r="B186" t="inlineStr">
         <is>
-          <t>2022-04-06</t>
+          <t>2022-04-18</t>
         </is>
       </c>
       <c r="C186" t="n">
@@ -2856,7 +2856,7 @@
       </c>
       <c r="B187" t="inlineStr">
         <is>
-          <t>2022-04-05</t>
+          <t>2022-04-17</t>
         </is>
       </c>
       <c r="C187" t="n">
@@ -2869,7 +2869,7 @@
       </c>
       <c r="B188" t="inlineStr">
         <is>
-          <t>2022-04-04</t>
+          <t>2022-04-14</t>
         </is>
       </c>
       <c r="C188" t="n">
@@ -2882,11 +2882,11 @@
       </c>
       <c r="B189" t="inlineStr">
         <is>
-          <t>2022-03-31</t>
+          <t>2022-04-12</t>
         </is>
       </c>
       <c r="C189" t="n">
-        <v>-0.4334</v>
+        <v>0.1198</v>
       </c>
     </row>
     <row r="190">
@@ -2895,11 +2895,11 @@
       </c>
       <c r="B190" t="inlineStr">
         <is>
-          <t>2022-03-29</t>
+          <t>2022-04-10</t>
         </is>
       </c>
       <c r="C190" t="n">
-        <v>0.2202</v>
+        <v>0</v>
       </c>
     </row>
     <row r="191">
@@ -2908,11 +2908,11 @@
       </c>
       <c r="B191" t="inlineStr">
         <is>
-          <t>2022-03-26</t>
+          <t>2022-04-08</t>
         </is>
       </c>
       <c r="C191" t="n">
-        <v>0.1012</v>
+        <v>0.1394</v>
       </c>
     </row>
     <row r="192">
@@ -2921,11 +2921,11 @@
       </c>
       <c r="B192" t="inlineStr">
         <is>
-          <t>2022-03-25</t>
+          <t>2022-04-07</t>
         </is>
       </c>
       <c r="C192" t="n">
-        <v>0.2023</v>
+        <v>0</v>
       </c>
     </row>
     <row r="193">
@@ -2934,11 +2934,11 @@
       </c>
       <c r="B193" t="inlineStr">
         <is>
-          <t>2022-03-24</t>
+          <t>2022-04-06</t>
         </is>
       </c>
       <c r="C193" t="n">
-        <v>0.1012</v>
+        <v>0</v>
       </c>
     </row>
     <row r="194">
@@ -2947,11 +2947,11 @@
       </c>
       <c r="B194" t="inlineStr">
         <is>
-          <t>2022-03-23</t>
+          <t>2022-04-05</t>
         </is>
       </c>
       <c r="C194" t="n">
-        <v>0.1012</v>
+        <v>0</v>
       </c>
     </row>
     <row r="195">
@@ -2960,11 +2960,11 @@
       </c>
       <c r="B195" t="inlineStr">
         <is>
-          <t>2022-03-21</t>
+          <t>2022-04-04</t>
         </is>
       </c>
       <c r="C195" t="n">
-        <v>0.0911</v>
+        <v>0</v>
       </c>
     </row>
     <row r="196">
@@ -2973,11 +2973,11 @@
       </c>
       <c r="B196" t="inlineStr">
         <is>
-          <t>2022-03-17</t>
+          <t>2022-03-31</t>
         </is>
       </c>
       <c r="C196" t="n">
-        <v>0.1012</v>
+        <v>-0.4334</v>
       </c>
     </row>
     <row r="197">
@@ -2986,11 +2986,11 @@
       </c>
       <c r="B197" t="inlineStr">
         <is>
-          <t>2022-03-16</t>
+          <t>2022-03-29</t>
         </is>
       </c>
       <c r="C197" t="n">
-        <v>0</v>
+        <v>0.2202</v>
       </c>
     </row>
     <row r="198">
@@ -2999,11 +2999,11 @@
       </c>
       <c r="B198" t="inlineStr">
         <is>
-          <t>2022-03-15</t>
+          <t>2022-03-26</t>
         </is>
       </c>
       <c r="C198" t="n">
-        <v>0.2023</v>
+        <v>0.1012</v>
       </c>
     </row>
     <row r="199">
@@ -3012,11 +3012,11 @@
       </c>
       <c r="B199" t="inlineStr">
         <is>
-          <t>2022-03-14</t>
+          <t>2022-03-25</t>
         </is>
       </c>
       <c r="C199" t="n">
-        <v>0.0674</v>
+        <v>0.2023</v>
       </c>
     </row>
     <row r="200">
@@ -3025,11 +3025,11 @@
       </c>
       <c r="B200" t="inlineStr">
         <is>
-          <t>2022-03-13</t>
+          <t>2022-03-24</t>
         </is>
       </c>
       <c r="C200" t="n">
-        <v>0</v>
+        <v>0.1012</v>
       </c>
     </row>
     <row r="201">
@@ -3038,11 +3038,11 @@
       </c>
       <c r="B201" t="inlineStr">
         <is>
-          <t>2022-03-12</t>
+          <t>2022-03-23</t>
         </is>
       </c>
       <c r="C201" t="n">
-        <v>0</v>
+        <v>0.1012</v>
       </c>
     </row>
     <row r="202">
@@ -3051,11 +3051,11 @@
       </c>
       <c r="B202" t="inlineStr">
         <is>
-          <t>2022-03-11</t>
+          <t>2022-03-21</t>
         </is>
       </c>
       <c r="C202" t="n">
-        <v>-0.0258</v>
+        <v>0.0911</v>
       </c>
     </row>
     <row r="203">
@@ -3064,11 +3064,11 @@
       </c>
       <c r="B203" t="inlineStr">
         <is>
-          <t>2022-03-10</t>
+          <t>2022-03-17</t>
         </is>
       </c>
       <c r="C203" t="n">
-        <v>0</v>
+        <v>0.1012</v>
       </c>
     </row>
     <row r="204">
@@ -3077,7 +3077,7 @@
       </c>
       <c r="B204" t="inlineStr">
         <is>
-          <t>2022-03-09</t>
+          <t>2022-03-16</t>
         </is>
       </c>
       <c r="C204" t="n">
@@ -3090,11 +3090,11 @@
       </c>
       <c r="B205" t="inlineStr">
         <is>
-          <t>2022-03-08</t>
+          <t>2022-03-15</t>
         </is>
       </c>
       <c r="C205" t="n">
-        <v>0</v>
+        <v>0.2023</v>
       </c>
     </row>
     <row r="206">
@@ -3103,11 +3103,11 @@
       </c>
       <c r="B206" t="inlineStr">
         <is>
-          <t>2022-03-07</t>
+          <t>2022-03-14</t>
         </is>
       </c>
       <c r="C206" t="n">
-        <v>0.0566</v>
+        <v>0.0674</v>
       </c>
     </row>
     <row r="207">
@@ -3116,7 +3116,7 @@
       </c>
       <c r="B207" t="inlineStr">
         <is>
-          <t>2022-03-06</t>
+          <t>2022-03-13</t>
         </is>
       </c>
       <c r="C207" t="n">
@@ -3129,11 +3129,11 @@
       </c>
       <c r="B208" t="inlineStr">
         <is>
-          <t>2022-03-05</t>
+          <t>2022-03-12</t>
         </is>
       </c>
       <c r="C208" t="n">
-        <v>0.5423</v>
+        <v>0</v>
       </c>
     </row>
     <row r="209">
@@ -3142,11 +3142,11 @@
       </c>
       <c r="B209" t="inlineStr">
         <is>
-          <t>2022-03-02</t>
+          <t>2022-03-11</t>
         </is>
       </c>
       <c r="C209" t="n">
-        <v>0.2482</v>
+        <v>-0.0258</v>
       </c>
     </row>
     <row r="210">
@@ -3155,11 +3155,11 @@
       </c>
       <c r="B210" t="inlineStr">
         <is>
-          <t>2022-03-01</t>
+          <t>2022-03-10</t>
         </is>
       </c>
       <c r="C210" t="n">
-        <v>0.0803</v>
+        <v>0</v>
       </c>
     </row>
     <row r="211">
@@ -3168,11 +3168,11 @@
       </c>
       <c r="B211" t="inlineStr">
         <is>
-          <t>2022-02-28</t>
+          <t>2022-03-09</t>
         </is>
       </c>
       <c r="C211" t="n">
-        <v>-0.3818</v>
+        <v>0</v>
       </c>
     </row>
     <row r="212">
@@ -3181,11 +3181,11 @@
       </c>
       <c r="B212" t="inlineStr">
         <is>
-          <t>2022-02-26</t>
+          <t>2022-03-08</t>
         </is>
       </c>
       <c r="C212" t="n">
-        <v>-0.3818</v>
+        <v>0</v>
       </c>
     </row>
     <row r="213">
@@ -3194,11 +3194,11 @@
       </c>
       <c r="B213" t="inlineStr">
         <is>
-          <t>2022-02-25</t>
+          <t>2022-03-07</t>
         </is>
       </c>
       <c r="C213" t="n">
-        <v>0</v>
+        <v>0.0566</v>
       </c>
     </row>
     <row r="214">
@@ -3207,11 +3207,11 @@
       </c>
       <c r="B214" t="inlineStr">
         <is>
-          <t>2022-02-24</t>
+          <t>2022-03-06</t>
         </is>
       </c>
       <c r="C214" t="n">
-        <v>0.0674</v>
+        <v>0</v>
       </c>
     </row>
     <row r="215">
@@ -3220,11 +3220,11 @@
       </c>
       <c r="B215" t="inlineStr">
         <is>
-          <t>2022-02-19</t>
+          <t>2022-03-05</t>
         </is>
       </c>
       <c r="C215" t="n">
-        <v>-0.0898</v>
+        <v>0.5423</v>
       </c>
     </row>
     <row r="216">
@@ -3233,11 +3233,11 @@
       </c>
       <c r="B216" t="inlineStr">
         <is>
-          <t>2022-02-17</t>
+          <t>2022-03-02</t>
         </is>
       </c>
       <c r="C216" t="n">
-        <v>0</v>
+        <v>0.2482</v>
       </c>
     </row>
     <row r="217">
@@ -3246,11 +3246,11 @@
       </c>
       <c r="B217" t="inlineStr">
         <is>
-          <t>2022-02-16</t>
+          <t>2022-03-01</t>
         </is>
       </c>
       <c r="C217" t="n">
-        <v>0</v>
+        <v>0.0803</v>
       </c>
     </row>
     <row r="218">
@@ -3259,11 +3259,11 @@
       </c>
       <c r="B218" t="inlineStr">
         <is>
-          <t>2022-02-15</t>
+          <t>2022-02-28</t>
         </is>
       </c>
       <c r="C218" t="n">
-        <v>0.1012</v>
+        <v>-0.3818</v>
       </c>
     </row>
     <row r="219">
@@ -3272,11 +3272,11 @@
       </c>
       <c r="B219" t="inlineStr">
         <is>
-          <t>2022-02-14</t>
+          <t>2022-02-26</t>
         </is>
       </c>
       <c r="C219" t="n">
-        <v>-0.0898</v>
+        <v>-0.3818</v>
       </c>
     </row>
     <row r="220">
@@ -3285,11 +3285,11 @@
       </c>
       <c r="B220" t="inlineStr">
         <is>
-          <t>2022-02-12</t>
+          <t>2022-02-25</t>
         </is>
       </c>
       <c r="C220" t="n">
-        <v>0.0674</v>
+        <v>0</v>
       </c>
     </row>
     <row r="221">
@@ -3298,11 +3298,11 @@
       </c>
       <c r="B221" t="inlineStr">
         <is>
-          <t>2022-02-11</t>
+          <t>2022-02-24</t>
         </is>
       </c>
       <c r="C221" t="n">
-        <v>-0.17</v>
+        <v>0.0674</v>
       </c>
     </row>
     <row r="222">
@@ -3311,11 +3311,11 @@
       </c>
       <c r="B222" t="inlineStr">
         <is>
-          <t>2022-02-10</t>
+          <t>2022-02-19</t>
         </is>
       </c>
       <c r="C222" t="n">
-        <v>0.0506</v>
+        <v>-0.0898</v>
       </c>
     </row>
     <row r="223">
@@ -3324,7 +3324,7 @@
       </c>
       <c r="B223" t="inlineStr">
         <is>
-          <t>2022-02-09</t>
+          <t>2022-02-17</t>
         </is>
       </c>
       <c r="C223" t="n">
@@ -3337,11 +3337,11 @@
       </c>
       <c r="B224" t="inlineStr">
         <is>
-          <t>2022-02-08</t>
+          <t>2022-02-16</t>
         </is>
       </c>
       <c r="C224" t="n">
-        <v>0.34</v>
+        <v>0</v>
       </c>
     </row>
     <row r="225">
@@ -3350,11 +3350,11 @@
       </c>
       <c r="B225" t="inlineStr">
         <is>
-          <t>2022-02-06</t>
+          <t>2022-02-15</t>
         </is>
       </c>
       <c r="C225" t="n">
-        <v>-0.3818</v>
+        <v>0.1012</v>
       </c>
     </row>
     <row r="226">
@@ -3363,11 +3363,11 @@
       </c>
       <c r="B226" t="inlineStr">
         <is>
-          <t>2022-02-04</t>
+          <t>2022-02-14</t>
         </is>
       </c>
       <c r="C226" t="n">
-        <v>0.0674</v>
+        <v>-0.0898</v>
       </c>
     </row>
     <row r="227">
@@ -3376,11 +3376,11 @@
       </c>
       <c r="B227" t="inlineStr">
         <is>
-          <t>2022-02-03</t>
+          <t>2022-02-12</t>
         </is>
       </c>
       <c r="C227" t="n">
-        <v>0.2023</v>
+        <v>0.0674</v>
       </c>
     </row>
     <row r="228">
@@ -3389,11 +3389,11 @@
       </c>
       <c r="B228" t="inlineStr">
         <is>
-          <t>2022-01-31</t>
+          <t>2022-02-11</t>
         </is>
       </c>
       <c r="C228" t="n">
-        <v>0.2023</v>
+        <v>-0.17</v>
       </c>
     </row>
     <row r="229">
@@ -3402,11 +3402,11 @@
       </c>
       <c r="B229" t="inlineStr">
         <is>
-          <t>2022-01-28</t>
+          <t>2022-02-10</t>
         </is>
       </c>
       <c r="C229" t="n">
-        <v>0.2023</v>
+        <v>0.0506</v>
       </c>
     </row>
     <row r="230">
@@ -3415,11 +3415,11 @@
       </c>
       <c r="B230" t="inlineStr">
         <is>
-          <t>2022-01-20</t>
+          <t>2022-02-09</t>
         </is>
       </c>
       <c r="C230" t="n">
-        <v>0.3515</v>
+        <v>0</v>
       </c>
     </row>
     <row r="231">
@@ -3428,11 +3428,11 @@
       </c>
       <c r="B231" t="inlineStr">
         <is>
-          <t>2022-01-18</t>
+          <t>2022-02-08</t>
         </is>
       </c>
       <c r="C231" t="n">
-        <v>0.2385</v>
+        <v>0.34</v>
       </c>
     </row>
     <row r="232">
@@ -3441,11 +3441,11 @@
       </c>
       <c r="B232" t="inlineStr">
         <is>
-          <t>2022-01-17</t>
+          <t>2022-02-06</t>
         </is>
       </c>
       <c r="C232" t="n">
-        <v>0</v>
+        <v>-0.3818</v>
       </c>
     </row>
     <row r="233">
@@ -3454,11 +3454,11 @@
       </c>
       <c r="B233" t="inlineStr">
         <is>
-          <t>2022-01-15</t>
+          <t>2022-02-04</t>
         </is>
       </c>
       <c r="C233" t="n">
-        <v>0.1012</v>
+        <v>0.0674</v>
       </c>
     </row>
     <row r="234">
@@ -3467,11 +3467,11 @@
       </c>
       <c r="B234" t="inlineStr">
         <is>
-          <t>2022-01-14</t>
+          <t>2022-02-03</t>
         </is>
       </c>
       <c r="C234" t="n">
-        <v>0.0253</v>
+        <v>0.2023</v>
       </c>
     </row>
     <row r="235">
@@ -3480,11 +3480,11 @@
       </c>
       <c r="B235" t="inlineStr">
         <is>
-          <t>2022-01-13</t>
+          <t>2022-01-31</t>
         </is>
       </c>
       <c r="C235" t="n">
-        <v>0.1012</v>
+        <v>0.2023</v>
       </c>
     </row>
     <row r="236">
@@ -3493,11 +3493,11 @@
       </c>
       <c r="B236" t="inlineStr">
         <is>
-          <t>2022-01-12</t>
+          <t>2022-01-28</t>
         </is>
       </c>
       <c r="C236" t="n">
-        <v>0.134</v>
+        <v>0.2023</v>
       </c>
     </row>
     <row r="237">
@@ -3506,11 +3506,11 @@
       </c>
       <c r="B237" t="inlineStr">
         <is>
-          <t>2022-01-08</t>
+          <t>2022-01-20</t>
         </is>
       </c>
       <c r="C237" t="n">
-        <v>0</v>
+        <v>0.3515</v>
       </c>
     </row>
     <row r="238">
@@ -3519,11 +3519,11 @@
       </c>
       <c r="B238" t="inlineStr">
         <is>
-          <t>2022-01-07</t>
+          <t>2022-01-18</t>
         </is>
       </c>
       <c r="C238" t="n">
-        <v>0.2023</v>
+        <v>0.2385</v>
       </c>
     </row>
     <row r="239">
@@ -3532,7 +3532,7 @@
       </c>
       <c r="B239" t="inlineStr">
         <is>
-          <t>2022-01-06</t>
+          <t>2022-01-17</t>
         </is>
       </c>
       <c r="C239" t="n">
@@ -3545,11 +3545,11 @@
       </c>
       <c r="B240" t="inlineStr">
         <is>
-          <t>2022-01-05</t>
+          <t>2022-01-15</t>
         </is>
       </c>
       <c r="C240" t="n">
-        <v>0</v>
+        <v>0.1012</v>
       </c>
     </row>
     <row r="241">
@@ -3558,11 +3558,11 @@
       </c>
       <c r="B241" t="inlineStr">
         <is>
-          <t>2022-01-04</t>
+          <t>2022-01-14</t>
         </is>
       </c>
       <c r="C241" t="n">
-        <v>0.0148</v>
+        <v>0.0253</v>
       </c>
     </row>
     <row r="242">
@@ -3571,11 +3571,11 @@
       </c>
       <c r="B242" t="inlineStr">
         <is>
-          <t>2022-01-03</t>
+          <t>2022-01-13</t>
         </is>
       </c>
       <c r="C242" t="n">
-        <v>0</v>
+        <v>0.1012</v>
       </c>
     </row>
     <row r="243">
@@ -3584,11 +3584,11 @@
       </c>
       <c r="B243" t="inlineStr">
         <is>
-          <t>2021-12-31</t>
+          <t>2022-01-12</t>
         </is>
       </c>
       <c r="C243" t="n">
-        <v>-0.5266999999999999</v>
+        <v>0.134</v>
       </c>
     </row>
     <row r="244">
@@ -3597,7 +3597,7 @@
       </c>
       <c r="B244" t="inlineStr">
         <is>
-          <t>2021-12-29</t>
+          <t>2022-01-08</t>
         </is>
       </c>
       <c r="C244" t="n">
@@ -3610,11 +3610,11 @@
       </c>
       <c r="B245" t="inlineStr">
         <is>
-          <t>2021-12-27</t>
+          <t>2022-01-07</t>
         </is>
       </c>
       <c r="C245" t="n">
-        <v>0.5042</v>
+        <v>0.2023</v>
       </c>
     </row>
     <row r="246">
@@ -3623,7 +3623,7 @@
       </c>
       <c r="B246" t="inlineStr">
         <is>
-          <t>2021-12-26</t>
+          <t>2022-01-06</t>
         </is>
       </c>
       <c r="C246" t="n">
@@ -3636,7 +3636,7 @@
       </c>
       <c r="B247" t="inlineStr">
         <is>
-          <t>2021-12-25</t>
+          <t>2022-01-05</t>
         </is>
       </c>
       <c r="C247" t="n">
@@ -3649,11 +3649,11 @@
       </c>
       <c r="B248" t="inlineStr">
         <is>
-          <t>2021-12-22</t>
+          <t>2022-01-04</t>
         </is>
       </c>
       <c r="C248" t="n">
-        <v>0.1724</v>
+        <v>0.0148</v>
       </c>
     </row>
     <row r="249">
@@ -3662,10 +3662,101 @@
       </c>
       <c r="B249" t="inlineStr">
         <is>
+          <t>2022-01-03</t>
+        </is>
+      </c>
+      <c r="C249" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="250">
+      <c r="A250" s="1" t="n">
+        <v>248</v>
+      </c>
+      <c r="B250" t="inlineStr">
+        <is>
+          <t>2021-12-31</t>
+        </is>
+      </c>
+      <c r="C250" t="n">
+        <v>-0.5266999999999999</v>
+      </c>
+    </row>
+    <row r="251">
+      <c r="A251" s="1" t="n">
+        <v>249</v>
+      </c>
+      <c r="B251" t="inlineStr">
+        <is>
+          <t>2021-12-29</t>
+        </is>
+      </c>
+      <c r="C251" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="252">
+      <c r="A252" s="1" t="n">
+        <v>250</v>
+      </c>
+      <c r="B252" t="inlineStr">
+        <is>
+          <t>2021-12-27</t>
+        </is>
+      </c>
+      <c r="C252" t="n">
+        <v>0.5042</v>
+      </c>
+    </row>
+    <row r="253">
+      <c r="A253" s="1" t="n">
+        <v>251</v>
+      </c>
+      <c r="B253" t="inlineStr">
+        <is>
+          <t>2021-12-26</t>
+        </is>
+      </c>
+      <c r="C253" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="254">
+      <c r="A254" s="1" t="n">
+        <v>252</v>
+      </c>
+      <c r="B254" t="inlineStr">
+        <is>
+          <t>2021-12-25</t>
+        </is>
+      </c>
+      <c r="C254" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="255">
+      <c r="A255" s="1" t="n">
+        <v>253</v>
+      </c>
+      <c r="B255" t="inlineStr">
+        <is>
+          <t>2021-12-22</t>
+        </is>
+      </c>
+      <c r="C255" t="n">
+        <v>0.1724</v>
+      </c>
+    </row>
+    <row r="256">
+      <c r="A256" s="1" t="n">
+        <v>254</v>
+      </c>
+      <c r="B256" t="inlineStr">
+        <is>
           <t>2021-12-21</t>
         </is>
       </c>
-      <c r="C249" t="n">
+      <c r="C256" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>